<commit_message>
slight adjustment to plate reader data
</commit_message>
<xml_diff>
--- a/neutralization_assays/data/neut_plate_reader_data/557v1_NeutralizationAssay.xlsx
+++ b/neutralization_assays/data/neut_plate_reader_data/557v1_NeutralizationAssay.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39360" yWindow="7140" windowWidth="26840" windowHeight="11560" activeTab="3"/>
+    <workbookView xWindow="30820" yWindow="460" windowWidth="29020" windowHeight="17600"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
@@ -496,12 +496,6 @@
     <t>ms</t>
   </si>
   <si>
-    <t>Part of Plate</t>
-  </si>
-  <si>
-    <t>B1-G12</t>
-  </si>
-  <si>
     <t>Start Time:</t>
   </si>
   <si>
@@ -572,6 +566,12 @@
   </si>
   <si>
     <t>4/26/2019 10:03:06 AM</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -997,7 +997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1202,67 +1204,64 @@
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
+      <c r="B28" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="2" t="s">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>40</v>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>2</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
-        <v>4</v>
-      </c>
-      <c r="F32" s="3">
-        <v>5</v>
-      </c>
-      <c r="G32" s="3">
-        <v>6</v>
-      </c>
-      <c r="H32" s="3">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3">
-        <v>8</v>
-      </c>
-      <c r="J32" s="3">
-        <v>9</v>
-      </c>
-      <c r="K32" s="3">
-        <v>10</v>
-      </c>
-      <c r="L32" s="3">
-        <v>11</v>
-      </c>
-      <c r="M32" s="3">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>10356</v>
@@ -1303,7 +1302,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34">
         <v>30927</v>
@@ -1344,7 +1343,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>29530</v>
@@ -1385,7 +1384,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B36">
         <v>27904</v>
@@ -1426,7 +1425,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <v>26829</v>
@@ -1467,7 +1466,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38">
         <v>27396</v>
@@ -1506,12 +1505,17 @@
         <v>29391</v>
       </c>
     </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1525,7 +1529,7 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1567,7 +1571,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1731,67 +1735,64 @@
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>51</v>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>52</v>
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>2</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
-        <v>4</v>
-      </c>
-      <c r="F32" s="3">
-        <v>5</v>
-      </c>
-      <c r="G32" s="3">
-        <v>6</v>
-      </c>
-      <c r="H32" s="3">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3">
-        <v>8</v>
-      </c>
-      <c r="J32" s="3">
-        <v>9</v>
-      </c>
-      <c r="K32" s="3">
-        <v>10</v>
-      </c>
-      <c r="L32" s="3">
-        <v>11</v>
-      </c>
-      <c r="M32" s="3">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>6795</v>
@@ -1832,7 +1833,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34">
         <v>29042</v>
@@ -1873,7 +1874,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>28011</v>
@@ -1914,7 +1915,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B36">
         <v>26223</v>
@@ -1955,7 +1956,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <v>27772</v>
@@ -1996,7 +1997,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38">
         <v>25660</v>
@@ -2035,12 +2036,17 @@
         <v>27476</v>
       </c>
     </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2053,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2096,7 +2102,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2260,67 +2266,64 @@
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>55</v>
+      <c r="B28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>56</v>
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>2</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
-        <v>4</v>
-      </c>
-      <c r="F32" s="3">
-        <v>5</v>
-      </c>
-      <c r="G32" s="3">
-        <v>6</v>
-      </c>
-      <c r="H32" s="3">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3">
-        <v>8</v>
-      </c>
-      <c r="J32" s="3">
-        <v>9</v>
-      </c>
-      <c r="K32" s="3">
-        <v>10</v>
-      </c>
-      <c r="L32" s="3">
-        <v>11</v>
-      </c>
-      <c r="M32" s="3">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>8707</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34">
         <v>30244</v>
@@ -2402,7 +2405,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>28117</v>
@@ -2443,7 +2446,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B36">
         <v>25835</v>
@@ -2484,7 +2487,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <v>26975</v>
@@ -2525,7 +2528,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38">
         <v>25848</v>
@@ -2564,12 +2567,17 @@
         <v>27291</v>
       </c>
     </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2582,8 +2590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2625,7 +2633,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2789,67 +2797,64 @@
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>59</v>
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>60</v>
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>2</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
-        <v>4</v>
-      </c>
-      <c r="F32" s="3">
-        <v>5</v>
-      </c>
-      <c r="G32" s="3">
-        <v>6</v>
-      </c>
-      <c r="H32" s="3">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3">
-        <v>8</v>
-      </c>
-      <c r="J32" s="3">
-        <v>9</v>
-      </c>
-      <c r="K32" s="3">
-        <v>10</v>
-      </c>
-      <c r="L32" s="3">
-        <v>11</v>
-      </c>
-      <c r="M32" s="3">
-        <v>12</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B33">
         <v>10404</v>
@@ -2890,7 +2895,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B34">
         <v>32985</v>
@@ -2931,7 +2936,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B35">
         <v>30722</v>
@@ -2972,7 +2977,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B36">
         <v>30437</v>
@@ -3013,7 +3018,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <v>27147</v>
@@ -3054,7 +3059,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38">
         <v>25485</v>
@@ -3093,12 +3098,17 @@
         <v>20660</v>
       </c>
     </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>